<commit_message>
Dodane pliki z cwiczeniami gramatycznymi. Rozszerzone zbiory 2016-01. Poprawki w b-der-mensch
</commit_message>
<xml_diff>
--- a/wortschatz-m/2016-01.xlsx
+++ b/wortschatz-m/2016-01.xlsx
@@ -11,12 +11,12 @@
     <sheet name="Arkusz2" sheetId="2" r:id="rId2"/>
     <sheet name="Arkusz3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>e</t>
   </si>
@@ -28,18 +28,48 @@
   </si>
   <si>
     <t>Unverschämt!</t>
+  </si>
+  <si>
+    <t>Wir kommen gleich nach!</t>
+  </si>
+  <si>
+    <t>verdorben</t>
+  </si>
+  <si>
+    <t>ersticken</t>
+  </si>
+  <si>
+    <t>Gefallen tun</t>
+  </si>
+  <si>
+    <t>empören gegen</t>
+  </si>
+  <si>
+    <t>hinrichten</t>
+  </si>
+  <si>
+    <t>das Übel an der Wurzel packen</t>
+  </si>
+  <si>
+    <t>Dolmetscher</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Czcionka tekstu podstawowego"/>
       <family val="2"/>
+      <charset val="238"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Czcionka tekstu podstawowego"/>
       <charset val="238"/>
     </font>
   </fonts>
@@ -63,8 +93,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -359,10 +390,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -387,6 +418,46 @@
     <row r="2" spans="1:3">
       <c r="B2" t="s">
         <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="B8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="B9" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="B10" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>